<commit_message>
debugging browser on output of user new plot
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart (1).xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD59D04-F71A-45CE-84A0-E0D07F8BE72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734AE036-495E-4016-859B-AA90907301A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="3720" windowWidth="11460" windowHeight="11340" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -995,6 +995,13 @@
     <xf numFmtId="0" fontId="27" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1007,13 +1014,6 @@
     <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1584,7 +1584,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1629,118 +1629,118 @@
       <c r="B3" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="92"/>
-      <c r="E3" s="90">
+      <c r="D3" s="88"/>
+      <c r="E3" s="93">
         <f ca="1">TODAY()</f>
-        <v>45039</v>
-      </c>
-      <c r="F3" s="90"/>
+        <v>45043</v>
+      </c>
+      <c r="F3" s="93"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="88"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="87">
+      <c r="I4" s="90">
         <f ca="1">I5</f>
         <v>45040</v>
       </c>
-      <c r="J4" s="88"/>
-      <c r="K4" s="88"/>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87">
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="92"/>
+      <c r="P4" s="90">
         <f ca="1">P5</f>
         <v>45047</v>
       </c>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="87">
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
+      <c r="S4" s="91"/>
+      <c r="T4" s="91"/>
+      <c r="U4" s="91"/>
+      <c r="V4" s="92"/>
+      <c r="W4" s="90">
         <f ca="1">W5</f>
         <v>45054</v>
       </c>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="88"/>
-      <c r="AB4" s="88"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="87">
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="92"/>
+      <c r="AD4" s="90">
         <f ca="1">AD5</f>
         <v>45061</v>
       </c>
-      <c r="AE4" s="88"/>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="88"/>
-      <c r="AH4" s="88"/>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="87">
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="92"/>
+      <c r="AK4" s="90">
         <f ca="1">AK5</f>
         <v>45068</v>
       </c>
-      <c r="AL4" s="88"/>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="88"/>
-      <c r="AO4" s="88"/>
-      <c r="AP4" s="88"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="87">
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+      <c r="AN4" s="91"/>
+      <c r="AO4" s="91"/>
+      <c r="AP4" s="91"/>
+      <c r="AQ4" s="92"/>
+      <c r="AR4" s="90">
         <f ca="1">AR5</f>
         <v>45075</v>
       </c>
-      <c r="AS4" s="88"/>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="88"/>
-      <c r="AV4" s="88"/>
-      <c r="AW4" s="88"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="87">
+      <c r="AS4" s="91"/>
+      <c r="AT4" s="91"/>
+      <c r="AU4" s="91"/>
+      <c r="AV4" s="91"/>
+      <c r="AW4" s="91"/>
+      <c r="AX4" s="92"/>
+      <c r="AY4" s="90">
         <f ca="1">AY5</f>
         <v>45082</v>
       </c>
-      <c r="AZ4" s="88"/>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="88"/>
-      <c r="BC4" s="88"/>
-      <c r="BD4" s="88"/>
-      <c r="BE4" s="89"/>
-      <c r="BF4" s="87">
+      <c r="AZ4" s="91"/>
+      <c r="BA4" s="91"/>
+      <c r="BB4" s="91"/>
+      <c r="BC4" s="91"/>
+      <c r="BD4" s="91"/>
+      <c r="BE4" s="92"/>
+      <c r="BF4" s="90">
         <f ca="1">BF5</f>
         <v>45089</v>
       </c>
-      <c r="BG4" s="88"/>
-      <c r="BH4" s="88"/>
-      <c r="BI4" s="88"/>
-      <c r="BJ4" s="88"/>
-      <c r="BK4" s="88"/>
-      <c r="BL4" s="89"/>
+      <c r="BG4" s="91"/>
+      <c r="BH4" s="91"/>
+      <c r="BI4" s="91"/>
+      <c r="BJ4" s="91"/>
+      <c r="BK4" s="91"/>
+      <c r="BL4" s="92"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="93"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="93"/>
-      <c r="F5" s="93"/>
-      <c r="G5" s="93"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
       <c r="I5" s="11">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>45040</v>
@@ -3739,7 +3739,7 @@
         <v>47</v>
       </c>
       <c r="D27" s="37">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E27" s="65">
         <v>45020</v>
@@ -4542,11 +4542,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4554,6 +4549,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <conditionalFormatting sqref="D7:D34">

</xml_diff>

<commit_message>
Update Medical Al Disease Diagnostic Tool.Gantt.Chart (1).xlsx
</commit_message>
<xml_diff>
--- a/Medical Al Disease Diagnostic Tool.Gantt.Chart (1).xlsx
+++ b/Medical Al Disease Diagnostic Tool.Gantt.Chart (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166B7F58-4F80-499F-A649-602D86CE5836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D77AB2-E0D3-458C-8142-42098DA0377C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30615" yWindow="405" windowWidth="26925" windowHeight="15390" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1875" yWindow="210" windowWidth="26925" windowHeight="15390" tabRatio="426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -295,9 +295,6 @@
     <t>TensorFlow</t>
   </si>
   <si>
-    <t>Electronic Application</t>
-  </si>
-  <si>
     <t xml:space="preserve">Senior Project Poster </t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>Mansoor, Korie</t>
+  </si>
+  <si>
+    <t>Electron Application</t>
   </si>
 </sst>
 </file>
@@ -967,6 +967,25 @@
     <xf numFmtId="0" fontId="25" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="16" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -975,25 +994,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="16" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1595,7 +1595,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1647,189 +1647,189 @@
       <c r="B3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="76">
+      <c r="D3" s="77"/>
+      <c r="E3" s="79">
         <f ca="1">TODAY()</f>
-        <v>45045</v>
-      </c>
-      <c r="F3" s="76"/>
+        <v>45051</v>
+      </c>
+      <c r="F3" s="79"/>
     </row>
     <row r="4" spans="1:36" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="78"/>
+      <c r="D4" s="77"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="73">
+      <c r="I4" s="80">
         <f ca="1">I5</f>
-        <v>45040</v>
-      </c>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="74"/>
-      <c r="N4" s="74"/>
-      <c r="O4" s="75"/>
-      <c r="P4" s="73">
+        <v>45047</v>
+      </c>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="80">
         <f ca="1">P5</f>
-        <v>45047</v>
-      </c>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="74"/>
-      <c r="S4" s="74"/>
-      <c r="T4" s="74"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="75"/>
-      <c r="W4" s="73">
+        <v>45054</v>
+      </c>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="80">
         <f ca="1">W5</f>
-        <v>45054</v>
-      </c>
-      <c r="X4" s="74"/>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
-      <c r="AA4" s="74"/>
-      <c r="AB4" s="74"/>
-      <c r="AC4" s="75"/>
-      <c r="AD4" s="73">
+        <v>45061</v>
+      </c>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="82"/>
+      <c r="AD4" s="80">
         <f ca="1">AD5</f>
-        <v>45061</v>
-      </c>
-      <c r="AE4" s="74"/>
-      <c r="AF4" s="74"/>
-      <c r="AG4" s="74"/>
-      <c r="AH4" s="74"/>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="75"/>
+        <v>45068</v>
+      </c>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="81"/>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="82"/>
     </row>
     <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
       <c r="I5" s="10">
         <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45040</v>
+        <v>45047</v>
       </c>
       <c r="J5" s="9">
         <f ca="1">I5+1</f>
-        <v>45041</v>
+        <v>45048</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" ref="K5:AJ5" ca="1" si="0">J5+1</f>
-        <v>45042</v>
+        <v>45049</v>
       </c>
       <c r="L5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45043</v>
+        <v>45050</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45044</v>
+        <v>45051</v>
       </c>
       <c r="N5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45045</v>
+        <v>45052</v>
       </c>
       <c r="O5" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>45046</v>
+        <v>45053</v>
       </c>
       <c r="P5" s="10">
         <f ca="1">O5+1</f>
-        <v>45047</v>
+        <v>45054</v>
       </c>
       <c r="Q5" s="9">
         <f ca="1">P5+1</f>
-        <v>45048</v>
+        <v>45055</v>
       </c>
       <c r="R5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45049</v>
+        <v>45056</v>
       </c>
       <c r="S5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45050</v>
+        <v>45057</v>
       </c>
       <c r="T5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45051</v>
+        <v>45058</v>
       </c>
       <c r="U5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45052</v>
+        <v>45059</v>
       </c>
       <c r="V5" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>45053</v>
+        <v>45060</v>
       </c>
       <c r="W5" s="10">
         <f ca="1">V5+1</f>
-        <v>45054</v>
+        <v>45061</v>
       </c>
       <c r="X5" s="9">
         <f ca="1">W5+1</f>
-        <v>45055</v>
+        <v>45062</v>
       </c>
       <c r="Y5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45056</v>
+        <v>45063</v>
       </c>
       <c r="Z5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45057</v>
+        <v>45064</v>
       </c>
       <c r="AA5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45058</v>
+        <v>45065</v>
       </c>
       <c r="AB5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45059</v>
+        <v>45066</v>
       </c>
       <c r="AC5" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>45060</v>
+        <v>45067</v>
       </c>
       <c r="AD5" s="10">
         <f ca="1">AC5+1</f>
-        <v>45061</v>
+        <v>45068</v>
       </c>
       <c r="AE5" s="9">
         <f ca="1">AD5+1</f>
-        <v>45062</v>
+        <v>45069</v>
       </c>
       <c r="AF5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45063</v>
+        <v>45070</v>
       </c>
       <c r="AG5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45064</v>
+        <v>45071</v>
       </c>
       <c r="AH5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45065</v>
+        <v>45072</v>
       </c>
       <c r="AI5" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>45066</v>
+        <v>45073</v>
       </c>
       <c r="AJ5" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>45067</v>
+        <v>45074</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3272,7 +3272,7 @@
       <c r="C34" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="81">
+      <c r="D34" s="74">
         <v>1</v>
       </c>
       <c r="E34" s="54">
@@ -3283,20 +3283,20 @@
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
-      <c r="I34" s="82"/>
-      <c r="J34" s="82"/>
-      <c r="K34" s="82"/>
-      <c r="L34" s="82"/>
-      <c r="M34" s="82"/>
-      <c r="N34" s="82"/>
-      <c r="O34" s="82"/>
-      <c r="P34" s="82"/>
-      <c r="Q34" s="82"/>
-      <c r="R34" s="82"/>
-      <c r="S34" s="82"/>
-      <c r="T34" s="82"/>
-      <c r="U34" s="82"/>
-      <c r="V34" s="82"/>
+      <c r="I34" s="75"/>
+      <c r="J34" s="75"/>
+      <c r="K34" s="75"/>
+      <c r="L34" s="75"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
+      <c r="R34" s="75"/>
+      <c r="S34" s="75"/>
+      <c r="T34" s="75"/>
+      <c r="U34" s="75"/>
+      <c r="V34" s="75"/>
       <c r="W34" s="35"/>
       <c r="X34" s="35"/>
       <c r="Y34" s="35"/>
@@ -3315,7 +3315,7 @@
     <row r="35" spans="1:36" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="47"/>
       <c r="B35" s="69" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C35" s="61" t="s">
         <v>47</v>
@@ -3331,20 +3331,20 @@
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="80"/>
-      <c r="U35" s="80"/>
-      <c r="V35" s="80"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="73"/>
+      <c r="Q35" s="73"/>
+      <c r="R35" s="73"/>
+      <c r="S35" s="73"/>
+      <c r="T35" s="73"/>
+      <c r="U35" s="73"/>
+      <c r="V35" s="73"/>
       <c r="W35" s="35"/>
       <c r="X35" s="35"/>
       <c r="Y35" s="35"/>
@@ -3365,10 +3365,10 @@
         <v>25</v>
       </c>
       <c r="B36" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="61" t="s">
         <v>78</v>
-      </c>
-      <c r="C36" s="61" t="s">
-        <v>79</v>
       </c>
       <c r="D36" s="34">
         <v>1</v>
@@ -3381,20 +3381,20 @@
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
-      <c r="K36" s="80"/>
-      <c r="L36" s="80"/>
-      <c r="M36" s="80"/>
-      <c r="N36" s="80"/>
-      <c r="O36" s="80"/>
-      <c r="P36" s="80"/>
-      <c r="Q36" s="80"/>
-      <c r="R36" s="80"/>
-      <c r="S36" s="80"/>
-      <c r="T36" s="80"/>
-      <c r="U36" s="80"/>
-      <c r="V36" s="80"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+      <c r="Q36" s="73"/>
+      <c r="R36" s="73"/>
+      <c r="S36" s="73"/>
+      <c r="T36" s="73"/>
+      <c r="U36" s="73"/>
+      <c r="V36" s="73"/>
       <c r="W36" s="35"/>
       <c r="X36" s="35"/>
       <c r="Y36" s="35"/>
@@ -3434,20 +3434,20 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I37" s="80"/>
-      <c r="J37" s="80"/>
-      <c r="K37" s="80"/>
-      <c r="L37" s="80"/>
-      <c r="M37" s="80"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="80"/>
-      <c r="Q37" s="80"/>
-      <c r="R37" s="80"/>
-      <c r="S37" s="80"/>
-      <c r="T37" s="80"/>
-      <c r="U37" s="80"/>
-      <c r="V37" s="80"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73"/>
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
       <c r="W37" s="35"/>
       <c r="X37" s="35"/>
       <c r="Y37" s="35"/>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="38" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="61" t="s">
         <v>50</v>
@@ -3484,20 +3484,20 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="I38" s="80"/>
-      <c r="J38" s="80"/>
-      <c r="K38" s="80"/>
-      <c r="L38" s="80"/>
-      <c r="M38" s="80"/>
-      <c r="N38" s="80"/>
-      <c r="O38" s="80"/>
-      <c r="P38" s="80"/>
-      <c r="Q38" s="80"/>
-      <c r="R38" s="80"/>
-      <c r="S38" s="80"/>
-      <c r="T38" s="80"/>
-      <c r="U38" s="80"/>
-      <c r="V38" s="80"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="73"/>
+      <c r="L38" s="73"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="73"/>
+      <c r="O38" s="73"/>
+      <c r="P38" s="73"/>
+      <c r="Q38" s="73"/>
+      <c r="R38" s="73"/>
+      <c r="S38" s="73"/>
+      <c r="T38" s="73"/>
+      <c r="U38" s="73"/>
+      <c r="V38" s="73"/>
       <c r="W38" s="35"/>
       <c r="X38" s="35"/>
       <c r="Y38" s="35"/>
@@ -3531,20 +3531,20 @@
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="80"/>
-      <c r="N39" s="80"/>
-      <c r="O39" s="80"/>
-      <c r="P39" s="80"/>
-      <c r="Q39" s="80"/>
-      <c r="R39" s="80"/>
-      <c r="S39" s="80"/>
-      <c r="T39" s="80"/>
-      <c r="U39" s="80"/>
-      <c r="V39" s="80"/>
+      <c r="I39" s="73"/>
+      <c r="J39" s="73"/>
+      <c r="K39" s="73"/>
+      <c r="L39" s="73"/>
+      <c r="M39" s="73"/>
+      <c r="N39" s="73"/>
+      <c r="O39" s="73"/>
+      <c r="P39" s="73"/>
+      <c r="Q39" s="73"/>
+      <c r="R39" s="73"/>
+      <c r="S39" s="73"/>
+      <c r="T39" s="73"/>
+      <c r="U39" s="73"/>
+      <c r="V39" s="73"/>
       <c r="W39" s="35"/>
       <c r="X39" s="35"/>
       <c r="Y39" s="35"/>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="40" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" s="61" t="s">
         <v>39</v>
@@ -3578,20 +3578,20 @@
       </c>
       <c r="G40" s="14"/>
       <c r="H40" s="14"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="80"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="80"/>
-      <c r="P40" s="80"/>
-      <c r="Q40" s="80"/>
-      <c r="R40" s="80"/>
-      <c r="S40" s="80"/>
-      <c r="T40" s="80"/>
-      <c r="U40" s="80"/>
-      <c r="V40" s="80"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="73"/>
+      <c r="P40" s="73"/>
+      <c r="Q40" s="73"/>
+      <c r="R40" s="73"/>
+      <c r="S40" s="73"/>
+      <c r="T40" s="73"/>
+      <c r="U40" s="73"/>
+      <c r="V40" s="73"/>
       <c r="W40" s="35"/>
       <c r="X40" s="35"/>
       <c r="Y40" s="35"/>
@@ -3609,10 +3609,10 @@
     </row>
     <row r="41" spans="1:36" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="61" t="s">
         <v>76</v>
-      </c>
-      <c r="C41" s="61" t="s">
-        <v>77</v>
       </c>
       <c r="D41" s="34">
         <v>1</v>
@@ -3625,20 +3625,20 @@
       </c>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
-      <c r="I41" s="80"/>
-      <c r="J41" s="80"/>
-      <c r="K41" s="80"/>
-      <c r="L41" s="80"/>
-      <c r="M41" s="80"/>
-      <c r="N41" s="80"/>
-      <c r="O41" s="80"/>
-      <c r="P41" s="80"/>
-      <c r="Q41" s="80"/>
-      <c r="R41" s="80"/>
-      <c r="S41" s="80"/>
-      <c r="T41" s="80"/>
-      <c r="U41" s="80"/>
-      <c r="V41" s="80"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="73"/>
+      <c r="O41" s="73"/>
+      <c r="P41" s="73"/>
+      <c r="Q41" s="73"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="73"/>
+      <c r="U41" s="73"/>
+      <c r="V41" s="73"/>
       <c r="W41" s="35"/>
       <c r="X41" s="35"/>
       <c r="Y41" s="35"/>
@@ -3656,14 +3656,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AC4"/>
-    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <conditionalFormatting sqref="D7:D41">

</xml_diff>